<commit_message>
Suffixing duplicated header names by default, support for print titles
</commit_message>
<xml_diff>
--- a/docs/examples/fruit_lovers.xlsx
+++ b/docs/examples/fruit_lovers.xlsx
@@ -9,7 +9,9 @@
     <sheet name="persons" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName localSheetId="0" name="_xlnm.Print_Titles">persons!1:2</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -62,17 +64,17 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font/>
+    <font>
+      <color rgb="FF777777"/>
+    </font>
     <font>
       <b val="1"/>
       <color rgb="FFFFFFFF"/>
     </font>
     <font>
-      <color rgb="FF777777"/>
-    </font>
-    <font>
       <sz val="20"/>
     </font>
+    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -101,31 +103,31 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="6">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="6"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="5">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
-    <cellStyle hidden="0" name="Row" xfId="1"/>
+    <cellStyle hidden="0" name="Description" xfId="1"/>
     <cellStyle hidden="0" name="Header, center" xfId="2"/>
-    <cellStyle hidden="0" name="Header" xfId="3"/>
-    <cellStyle hidden="0" name="Description" xfId="4"/>
-    <cellStyle hidden="0" name="Title" xfId="5"/>
-    <cellStyle hidden="0" name="Row, date" xfId="6"/>
+    <cellStyle hidden="0" name="Title" xfId="3"/>
+    <cellStyle hidden="0" name="Header" xfId="4"/>
+    <cellStyle hidden="0" name="Row, date" xfId="5"/>
+    <cellStyle hidden="0" name="Row" xfId="6"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -496,9 +498,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="D3:D4" type="list">
       <formula1>"Apple,Banana,Orange"</formula1>

</xml_diff>

<commit_message>
default style set vertically aligned to top
</commit_message>
<xml_diff>
--- a/docs/examples/fruit_lovers.xlsx
+++ b/docs/examples/fruit_lovers.xlsx
@@ -65,14 +65,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="20"/>
+    </font>
+    <font>
       <color rgb="FF777777"/>
     </font>
     <font>
       <b val="1"/>
       <color rgb="FFFFFFFF"/>
-    </font>
-    <font>
-      <sz val="20"/>
     </font>
     <font/>
   </fonts>
@@ -102,31 +102,37 @@
   <cellStyleXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="164"/>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="6"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="5">
-      <alignment horizontal="center"/>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="6">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="4">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
-    <cellStyle hidden="0" name="Description" xfId="1"/>
-    <cellStyle hidden="0" name="Header, center" xfId="2"/>
-    <cellStyle hidden="0" name="Title" xfId="3"/>
-    <cellStyle hidden="0" name="Header" xfId="4"/>
-    <cellStyle hidden="0" name="Row, date" xfId="5"/>
+    <cellStyle hidden="0" name="Title" xfId="1"/>
+    <cellStyle hidden="0" name="Description" xfId="2"/>
+    <cellStyle hidden="0" name="Header, center" xfId="3"/>
+    <cellStyle hidden="0" name="Row, date" xfId="4"/>
+    <cellStyle hidden="0" name="Header" xfId="5"/>
     <cellStyle hidden="0" name="Row" xfId="6"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>

</xml_diff>

<commit_message>
Bugfix: handle empty tables
</commit_message>
<xml_diff>
--- a/docs/examples/fruit_lovers.xlsx
+++ b/docs/examples/fruit_lovers.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>List of fruit lovers</t>
   </si>
@@ -33,21 +33,6 @@
   <si>
     <t>favorite_fruit</t>
   </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>Banana</t>
-  </si>
-  <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>Apple</t>
-  </si>
 </sst>
 </file>
 
@@ -64,17 +49,17 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font/>
     <font>
       <sz val="20"/>
-    </font>
-    <font>
-      <color rgb="FF777777"/>
     </font>
     <font>
       <b val="1"/>
       <color rgb="FFFFFFFF"/>
     </font>
-    <font/>
+    <font>
+      <color rgb="FF777777"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -104,44 +89,38 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164"/>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="6">
       <alignment vertical="top"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="6">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="4">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
-    <cellStyle hidden="0" name="Title" xfId="1"/>
-    <cellStyle hidden="0" name="Description" xfId="2"/>
+    <cellStyle hidden="0" name="Row" xfId="1"/>
+    <cellStyle hidden="0" name="Title" xfId="2"/>
     <cellStyle hidden="0" name="Header, center" xfId="3"/>
-    <cellStyle hidden="0" name="Row, date" xfId="4"/>
-    <cellStyle hidden="0" name="Header" xfId="5"/>
-    <cellStyle hidden="0" name="Row" xfId="6"/>
+    <cellStyle hidden="0" name="Description" xfId="4"/>
+    <cellStyle hidden="0" name="Row, date" xfId="5"/>
+    <cellStyle hidden="0" name="Header" xfId="6"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="persons" headerRowCount="1" id="1" name="persons" ref="A2:D4">
-  <autoFilter ref="A2:D4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="persons" headerRowCount="1" id="1" name="persons" ref="A2:D3">
+  <autoFilter ref="A2:D3"/>
   <tableColumns count="4">
     <tableColumn id="1" name="first_name"/>
     <tableColumn id="2" name="last_name"/>
@@ -440,10 +419,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A3" ySplit="2"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
       <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -475,37 +454,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>33802</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>31473</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="D3:D4" type="list">
+    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="D2:D2" type="list">
       <formula1>"Apple,Banana,Orange"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Table Sheet breaking change: Ability to customize TableColumn behaviour based on a row_type determined by the TableSheet
</commit_message>
<xml_diff>
--- a/docs/examples/fruit_lovers.xlsx
+++ b/docs/examples/fruit_lovers.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>List of fruit lovers</t>
   </si>
@@ -32,6 +32,21 @@
   </si>
   <si>
     <t>favorite_fruit</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Apple</t>
   </si>
 </sst>
 </file>
@@ -49,13 +64,13 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
     <font/>
     <font>
       <sz val="20"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="FFFFFFFF"/>
     </font>
     <font>
       <color rgb="FF777777"/>
@@ -86,32 +101,38 @@
   </borders>
   <cellStyleXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164"/>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="4">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="6">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="6">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
-    <cellStyle hidden="0" name="Row" xfId="1"/>
-    <cellStyle hidden="0" name="Title" xfId="2"/>
-    <cellStyle hidden="0" name="Header, center" xfId="3"/>
-    <cellStyle hidden="0" name="Description" xfId="4"/>
-    <cellStyle hidden="0" name="Row, date" xfId="5"/>
+    <cellStyle hidden="0" name="Header, center" xfId="1"/>
+    <cellStyle hidden="0" name="Row" xfId="2"/>
+    <cellStyle hidden="0" name="Row, date" xfId="3"/>
+    <cellStyle hidden="0" name="Title" xfId="4"/>
+    <cellStyle hidden="0" name="Description" xfId="5"/>
     <cellStyle hidden="0" name="Header" xfId="6"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -119,8 +140,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="persons" headerRowCount="1" id="1" name="persons" ref="A2:D3">
-  <autoFilter ref="A2:D3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="persons" headerRowCount="1" id="1" name="persons" ref="A2:D4">
+  <autoFilter ref="A2:D4"/>
   <tableColumns count="4">
     <tableColumn id="1" name="first_name"/>
     <tableColumn id="2" name="last_name"/>
@@ -419,10 +440,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A3" ySplit="2"/>
       <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -454,12 +475,35 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>33802</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>31473</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="D2:D2" type="list">
-      <formula1>"Apple,Banana,Orange"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Reworked style handling. StyleSet now used to style cells. Allows adding styles directly via the columns including modifying default styles using an extended style.
</commit_message>
<xml_diff>
--- a/docs/examples/fruit_lovers.xlsx
+++ b/docs/examples/fruit_lovers.xlsx
@@ -56,7 +56,7 @@
   <numFmts count="1">
     <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -65,16 +65,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="20"/>
+    </font>
+    <font>
       <b val="1"/>
       <color rgb="FFFFFFFF"/>
     </font>
     <font/>
-    <font>
-      <sz val="20"/>
-    </font>
-    <font>
-      <color rgb="FF777777"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -99,41 +96,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="4">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="6">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="3">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="5">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
-    <cellStyle hidden="0" name="Header, center" xfId="1"/>
-    <cellStyle hidden="0" name="Row" xfId="2"/>
-    <cellStyle hidden="0" name="Row, date" xfId="3"/>
-    <cellStyle hidden="0" name="Title" xfId="4"/>
-    <cellStyle hidden="0" name="Description" xfId="5"/>
-    <cellStyle hidden="0" name="Header" xfId="6"/>
+    <cellStyle hidden="0" name="Title" xfId="1"/>
+    <cellStyle hidden="0" name="Header" xfId="2"/>
+    <cellStyle hidden="0" name="Header, center" xfId="3"/>
+    <cellStyle hidden="0" name="Row" xfId="4"/>
+    <cellStyle hidden="0" name="Row, date" xfId="5"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>

</xml_diff>